<commit_message>
modelagens step-by-step para todos os 5 modelos realizada
</commit_message>
<xml_diff>
--- a/Notebooks/vol_semanal.xlsx
+++ b/Notebooks/vol_semanal.xlsx
@@ -1,20 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilistocco/Documents/TCC 2 - Ônibus/BancoDados/Notebooks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCDFD8B-4781-C041-9B9E-5B0A57D7EA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensitivity Report 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$64</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$H$18</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$H$18</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$H$18</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet1!$H$19</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>day_of_week</t>
   </si>
@@ -24,15 +79,73 @@
   <si>
     <t>Volume</t>
   </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>pred</t>
+  </si>
+  <si>
+    <t>erro abs</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.66 Sensitivity Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [vol_semanal.xlsx]Sheet1</t>
+  </si>
+  <si>
+    <t>Report Created: 19/10/2022 16:58:26</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>$H$18</t>
+  </si>
+  <si>
+    <t>alpha Data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,6 +161,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -57,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -80,27 +208,176 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E58A0B8-8FE4-A4CA-290D-2A59EED7916F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8712200" y="3810000"/>
+          <a:ext cx="4445000" cy="1003300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{963AB359-4FC7-81BE-BDDA-78D5D2522D21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8712200" y="3810000"/>
+          <a:ext cx="3365500" cy="673100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -142,7 +419,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,9 +451,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,6 +503,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -383,14 +696,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03D1C3E-6FC5-644F-B3B6-7DB9B74C365C}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-67.538432328206113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,8 +835,74 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -414,8 +915,76 @@
       <c r="D2">
         <v>241</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44354</v>
+      </c>
+      <c r="I2">
+        <v>290</v>
+      </c>
+      <c r="J2">
+        <f>I2</f>
+        <v>290</v>
+      </c>
+      <c r="K2">
+        <f>ABS(I2-J2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>44348</v>
+      </c>
+      <c r="P2">
+        <v>139</v>
+      </c>
+      <c r="R2" s="1">
+        <v>27</v>
+      </c>
+      <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="T2" s="4">
+        <v>44349</v>
+      </c>
+      <c r="U2">
+        <v>290</v>
+      </c>
+      <c r="W2" s="1">
+        <v>40</v>
+      </c>
+      <c r="X2">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>44357</v>
+      </c>
+      <c r="Z2">
+        <v>291</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>52</v>
+      </c>
+      <c r="AC2">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>44358</v>
+      </c>
+      <c r="AE2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -428,8 +997,76 @@
       <c r="D3">
         <v>287</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44361</v>
+      </c>
+      <c r="I3">
+        <v>291</v>
+      </c>
+      <c r="J3" s="7">
+        <f>J2+$H$18*(I2-J2)</f>
+        <v>290</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K14" si="0">ABS(I3-J3)</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>44355</v>
+      </c>
+      <c r="P3">
+        <v>311</v>
+      </c>
+      <c r="R3" s="1">
+        <v>28</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3" s="4">
+        <v>44356</v>
+      </c>
+      <c r="U3">
+        <v>291</v>
+      </c>
+      <c r="W3" s="1">
+        <v>41</v>
+      </c>
+      <c r="X3">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>44364</v>
+      </c>
+      <c r="Z3">
+        <v>259</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>53</v>
+      </c>
+      <c r="AC3">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>44365</v>
+      </c>
+      <c r="AE3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -442,8 +1079,76 @@
       <c r="D4">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>44368</v>
+      </c>
+      <c r="I4">
+        <v>331</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" ref="J4:J14" si="1">J3+$H$18*(I3-J3)</f>
+        <v>290.03499815503244</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>40.96500184496756</v>
+      </c>
+      <c r="M4" s="1">
+        <v>15</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>44362</v>
+      </c>
+      <c r="P4">
+        <v>288</v>
+      </c>
+      <c r="R4" s="1">
+        <v>29</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4" s="4">
+        <v>44363</v>
+      </c>
+      <c r="U4">
+        <v>331</v>
+      </c>
+      <c r="W4" s="1">
+        <v>42</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>44371</v>
+      </c>
+      <c r="Z4">
+        <v>277</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>54</v>
+      </c>
+      <c r="AC4">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>44372</v>
+      </c>
+      <c r="AE4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -456,8 +1161,76 @@
       <c r="D5">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>44375</v>
+      </c>
+      <c r="I5">
+        <v>110</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="1"/>
+        <v>291.46869764050746</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>181.46869764050746</v>
+      </c>
+      <c r="M5" s="1">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>44369</v>
+      </c>
+      <c r="P5">
+        <v>110</v>
+      </c>
+      <c r="R5" s="1">
+        <v>30</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5" s="4">
+        <v>44370</v>
+      </c>
+      <c r="U5">
+        <v>110</v>
+      </c>
+      <c r="W5" s="1">
+        <v>43</v>
+      </c>
+      <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>44378</v>
+      </c>
+      <c r="Z5">
+        <v>120</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>55</v>
+      </c>
+      <c r="AC5">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>44379</v>
+      </c>
+      <c r="AE5">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -470,8 +1243,76 @@
       <c r="D6">
         <v>256</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>44382</v>
+      </c>
+      <c r="I6">
+        <v>89</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>285.1176280269471</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>196.1176280269471</v>
+      </c>
+      <c r="M6" s="1">
+        <v>17</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>44376</v>
+      </c>
+      <c r="P6">
+        <v>107</v>
+      </c>
+      <c r="R6" s="1">
+        <v>31</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+      <c r="T6" s="4">
+        <v>44377</v>
+      </c>
+      <c r="U6">
+        <v>89</v>
+      </c>
+      <c r="W6" s="1">
+        <v>44</v>
+      </c>
+      <c r="X6">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>44385</v>
+      </c>
+      <c r="Z6">
+        <v>143</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>56</v>
+      </c>
+      <c r="AC6">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>44393</v>
+      </c>
+      <c r="AE6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -484,8 +1325,76 @@
       <c r="D7">
         <v>278</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>44389</v>
+      </c>
+      <c r="I7">
+        <v>271</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>278.25387287666251</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>7.2538728766625127</v>
+      </c>
+      <c r="M7" s="1">
+        <v>18</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>44383</v>
+      </c>
+      <c r="P7">
+        <v>260</v>
+      </c>
+      <c r="R7" s="1">
+        <v>32</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7" s="4">
+        <v>44384</v>
+      </c>
+      <c r="U7">
+        <v>271</v>
+      </c>
+      <c r="W7" s="1">
+        <v>45</v>
+      </c>
+      <c r="X7">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>44392</v>
+      </c>
+      <c r="Z7">
+        <v>301</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>57</v>
+      </c>
+      <c r="AC7">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>44400</v>
+      </c>
+      <c r="AE7">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -498,8 +1407,76 @@
       <c r="D8">
         <v>284</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>44396</v>
+      </c>
+      <c r="I8">
+        <v>278</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>278.00000070913933</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>7.091393285918457E-7</v>
+      </c>
+      <c r="M8" s="1">
+        <v>19</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
+        <v>44390</v>
+      </c>
+      <c r="P8">
+        <v>156</v>
+      </c>
+      <c r="R8" s="1">
+        <v>33</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8" s="4">
+        <v>44391</v>
+      </c>
+      <c r="U8">
+        <v>278</v>
+      </c>
+      <c r="W8" s="1">
+        <v>46</v>
+      </c>
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>44399</v>
+      </c>
+      <c r="Z8">
+        <v>285</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>58</v>
+      </c>
+      <c r="AC8">
+        <v>4</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>44407</v>
+      </c>
+      <c r="AE8">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -512,8 +1489,76 @@
       <c r="D9">
         <v>267</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>44403</v>
+      </c>
+      <c r="I9">
+        <v>217</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>278.00000068432075</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>61.000000684320753</v>
+      </c>
+      <c r="M9" s="1">
+        <v>20</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <v>44397</v>
+      </c>
+      <c r="P9">
+        <v>273</v>
+      </c>
+      <c r="R9" s="1">
+        <v>34</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9" s="4">
+        <v>44398</v>
+      </c>
+      <c r="U9">
+        <v>217</v>
+      </c>
+      <c r="W9" s="1">
+        <v>47</v>
+      </c>
+      <c r="X9">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>44406</v>
+      </c>
+      <c r="Z9">
+        <v>163</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>59</v>
+      </c>
+      <c r="AC9">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>44414</v>
+      </c>
+      <c r="AE9">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -526,8 +1571,76 @@
       <c r="D10">
         <v>288</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>44410</v>
+      </c>
+      <c r="I10">
+        <v>82</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>275.86511320339099</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>193.86511320339099</v>
+      </c>
+      <c r="M10" s="1">
+        <v>21</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="4">
+        <v>44404</v>
+      </c>
+      <c r="P10">
+        <v>359</v>
+      </c>
+      <c r="R10" s="1">
+        <v>35</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10" s="4">
+        <v>44405</v>
+      </c>
+      <c r="U10">
+        <v>82</v>
+      </c>
+      <c r="W10" s="1">
+        <v>48</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>44413</v>
+      </c>
+      <c r="Z10">
+        <v>81</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>60</v>
+      </c>
+      <c r="AC10">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>44421</v>
+      </c>
+      <c r="AE10">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -540,8 +1653,76 @@
       <c r="D11">
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>44417</v>
+      </c>
+      <c r="I11">
+        <v>295</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>269.08019191611407</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>25.919808083885925</v>
+      </c>
+      <c r="M11" s="1">
+        <v>22</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4">
+        <v>44411</v>
+      </c>
+      <c r="P11">
+        <v>297</v>
+      </c>
+      <c r="R11" s="1">
+        <v>36</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11" s="4">
+        <v>44412</v>
+      </c>
+      <c r="U11">
+        <v>295</v>
+      </c>
+      <c r="W11" s="1">
+        <v>49</v>
+      </c>
+      <c r="X11">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>44420</v>
+      </c>
+      <c r="Z11">
+        <v>268</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>61</v>
+      </c>
+      <c r="AC11">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>44428</v>
+      </c>
+      <c r="AE11">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -554,8 +1735,76 @@
       <c r="D12">
         <v>222</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>44424</v>
+      </c>
+      <c r="I12">
+        <v>330</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>269.98733737784539</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>60.012662622154608</v>
+      </c>
+      <c r="M12" s="1">
+        <v>23</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4">
+        <v>44418</v>
+      </c>
+      <c r="P12">
+        <v>114</v>
+      </c>
+      <c r="R12" s="1">
+        <v>37</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12" s="4">
+        <v>44419</v>
+      </c>
+      <c r="U12">
+        <v>330</v>
+      </c>
+      <c r="W12" s="1">
+        <v>50</v>
+      </c>
+      <c r="X12">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>44427</v>
+      </c>
+      <c r="Z12">
+        <v>262</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>62</v>
+      </c>
+      <c r="AC12">
+        <v>4</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>44435</v>
+      </c>
+      <c r="AE12">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -568,8 +1817,64 @@
       <c r="D13">
         <v>318</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>44431</v>
+      </c>
+      <c r="I13">
+        <v>333</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>272.08766984820602</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>60.912330151793981</v>
+      </c>
+      <c r="M13" s="1">
+        <v>24</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4">
+        <v>44425</v>
+      </c>
+      <c r="P13">
+        <v>221</v>
+      </c>
+      <c r="R13" s="1">
+        <v>38</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="T13" s="4">
+        <v>44426</v>
+      </c>
+      <c r="U13">
+        <v>333</v>
+      </c>
+      <c r="W13" s="1">
+        <v>51</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>44434</v>
+      </c>
+      <c r="Z13">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -582,8 +1887,52 @@
       <c r="D14">
         <v>221</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" s="1">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>44438</v>
+      </c>
+      <c r="I14">
+        <v>244</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>274.21948902224665</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>30.219489022246648</v>
+      </c>
+      <c r="M14" s="1">
+        <v>25</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>44432</v>
+      </c>
+      <c r="P14">
+        <v>293</v>
+      </c>
+      <c r="R14" s="1">
+        <v>39</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="T14" s="4">
+        <v>44433</v>
+      </c>
+      <c r="U14">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -596,8 +1945,21 @@
       <c r="D15">
         <v>139</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="J15" s="7"/>
+      <c r="M15" s="1">
+        <v>26</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4">
+        <v>44439</v>
+      </c>
+      <c r="P15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -611,7 +1973,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -625,7 +1987,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -638,8 +2000,14 @@
       <c r="D18">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="6">
+        <v>3.4998155032455916E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -652,8 +2020,15 @@
       <c r="D19">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="6">
+        <f>AVERAGE(K2:K15)</f>
+        <v>66.056508066616686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -667,7 +2042,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -681,7 +2056,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -695,7 +2070,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -709,7 +2084,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -723,7 +2098,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -737,7 +2112,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -751,7 +2126,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -765,7 +2140,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -779,7 +2154,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -793,7 +2168,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -807,7 +2182,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -821,7 +2196,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -835,7 +2210,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -849,7 +2224,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -863,7 +2238,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -877,7 +2252,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -891,7 +2266,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -905,7 +2280,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -919,7 +2294,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -933,7 +2308,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -947,7 +2322,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -961,7 +2336,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -975,7 +2350,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -989,7 +2364,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1003,7 +2378,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1017,7 +2392,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1031,7 +2406,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1045,7 +2420,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1059,7 +2434,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1073,7 +2448,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1087,7 +2462,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1101,7 +2476,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1115,7 +2490,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1129,7 +2504,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1143,7 +2518,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1157,7 +2532,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1171,7 +2546,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1185,7 +2560,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1199,7 +2574,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1213,7 +2588,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1227,7 +2602,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1241,7 +2616,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1255,7 +2630,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1269,7 +2644,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1284,6 +2659,8 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>